<commit_message>
creación de consola de planificación
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="480" windowWidth="19800" windowHeight="7350" activeTab="2"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Reporte atrasos" sheetId="2" r:id="rId2"/>
-    <sheet name="Reporte planificación" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Reporte atrasos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Reporte planificación" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Reporte de atrasos</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Empleados encargados instalación</t>
+  </si>
+  <si>
+    <t>8 ;12 ;13</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -74,25 +80,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,47 +112,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -436,27 +410,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="30" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="20"/>
+    <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="3" min="3" width="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -475,23 +462,49 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>42824</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>42835</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="13" width="30" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="20"/>
+    <col customWidth="1" max="2" min="2" width="30"/>
+    <col customWidth="1" max="3" min="3" width="30"/>
+    <col customWidth="1" max="4" min="4" width="30"/>
+    <col customWidth="1" max="5" min="5" width="30"/>
+    <col customWidth="1" max="6" min="6" width="30"/>
+    <col customWidth="1" max="7" min="7" width="30"/>
+    <col customWidth="1" max="8" min="8" width="30"/>
+    <col customWidth="1" max="9" min="9" width="30"/>
+    <col customWidth="1" max="10" min="10" width="30"/>
+    <col customWidth="1" max="11" min="11" width="30"/>
+    <col customWidth="1" max="12" min="12" width="30"/>
+    <col customWidth="1" max="13" min="13" width="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -541,52 +554,170 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
+      <c r="A4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>42816</v>
-      </c>
-      <c r="C4" s="2">
-        <v>42816</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="2" t="n">
+        <v>42817</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>42822</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>42823</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>42828</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>42829</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>42832</v>
+      </c>
+      <c r="J4" t="n">
+        <v>7</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>42835</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>42835</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>42817</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>42823</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>42824</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>42830</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>42831</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>42837</v>
+      </c>
+      <c r="J5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>42838</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>42845</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>42817</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>42832</v>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>42817</v>
-      </c>
-      <c r="F4" s="2">
-        <v>42817</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>42818</v>
-      </c>
-      <c r="I4" s="2">
-        <v>42818</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4" s="2">
-        <v>42821</v>
-      </c>
-      <c r="L4" s="2">
-        <v>42821</v>
-      </c>
-      <c r="M4">
+      <c r="E6" s="2" t="n">
+        <v>42835</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>42852</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>42853</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>42871</v>
+      </c>
+      <c r="J6" t="n">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>42872</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>42884</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="D5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="B7" s="2" t="n">
+        <v>42823</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>42830</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>42831</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>42838</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>42842</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>42850</v>
+      </c>
+      <c r="J7" t="n">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>42851</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>42857</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mas tipos de restricciones en usuario
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -573,7 +573,7 @@
         <v>42828</v>
       </c>
       <c r="G4" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>42829</v>
@@ -582,7 +582,7 @@
         <v>42832</v>
       </c>
       <c r="J4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>42835</v>
@@ -614,7 +614,7 @@
         <v>42830</v>
       </c>
       <c r="G5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>42831</v>
@@ -623,7 +623,7 @@
         <v>42837</v>
       </c>
       <c r="J5" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>42838</v>

</xml_diff>

<commit_message>
consola no se cae en proyectos ni en tareas
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Reporte de atrasos</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +576,7 @@
         <v>42828</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>42829</v>
@@ -582,7 +585,7 @@
         <v>42832</v>
       </c>
       <c r="J4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K4" s="2" t="n">
         <v>42835</v>
@@ -614,7 +617,7 @@
         <v>42830</v>
       </c>
       <c r="G5" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>42831</v>
@@ -623,7 +626,7 @@
         <v>42837</v>
       </c>
       <c r="J5" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K5" s="2" t="n">
         <v>42838</v>
@@ -715,6 +718,47 @@
       </c>
       <c r="M7" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>42824</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>42830</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>42831</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>42837</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>42838</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>42846</v>
+      </c>
+      <c r="J8" t="n">
+        <v>7</v>
+      </c>
+      <c r="K8" s="2" t="n">
+        <v>42849</v>
+      </c>
+      <c r="L8" s="2" t="n">
+        <v>42852</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglos a getCostProject y otros
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
-  <bookViews>
-    <workbookView xWindow="330" yWindow="480" windowWidth="19800" windowHeight="7350" activeTab="2"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Reporte atrasos" sheetId="2" r:id="rId2"/>
-    <sheet name="Reporte planificación" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Reporte atrasos" sheetId="2" r:id="rId2"/>
+    <s:sheet name="Reporte planificación" sheetId="3" r:id="rId3"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Reporte de atrasos</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Empleados encargados instalación</t>
+  </si>
+  <si>
+    <t>8 ;12 ;13</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -74,25 +80,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color rgb="00000000"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,47 +116,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -436,27 +415,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="30" customWidth="1"/>
+    <col customWidth="1" width="20" min="1" max="1"/>
+    <col customWidth="1" width="30" min="2" max="2"/>
+    <col customWidth="1" width="30" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -475,23 +467,49 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>42824</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>42837</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="13" width="30" customWidth="1"/>
+    <col customWidth="1" width="20" min="1" max="1"/>
+    <col customWidth="1" width="30" min="2" max="2"/>
+    <col customWidth="1" width="30" min="3" max="3"/>
+    <col customWidth="1" width="30" min="4" max="4"/>
+    <col customWidth="1" width="30" min="5" max="5"/>
+    <col customWidth="1" width="30" min="6" max="6"/>
+    <col customWidth="1" width="30" min="7" max="7"/>
+    <col customWidth="1" width="30" min="8" max="8"/>
+    <col customWidth="1" width="30" min="9" max="9"/>
+    <col customWidth="1" width="30" min="10" max="10"/>
+    <col customWidth="1" width="30" min="11" max="11"/>
+    <col customWidth="1" width="30" min="12" max="12"/>
+    <col customWidth="1" width="30" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -541,52 +559,170 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
+      <c r="A4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>42816</v>
-      </c>
-      <c r="C4" s="2">
-        <v>42816</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="2" t="n">
+        <v>42821</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>42824</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>42825</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>42830</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>42831</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>42836</v>
+      </c>
+      <c r="J4" t="n">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>42837</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>42837</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>42821</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>42825</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>42828</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>42832</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>42835</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>42842</v>
+      </c>
+      <c r="J5" t="n">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>42843</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>42849</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>42821</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>42836</v>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
-        <v>42817</v>
-      </c>
-      <c r="F4" s="2">
-        <v>42817</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>42818</v>
-      </c>
-      <c r="I4" s="2">
-        <v>42818</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4" s="2">
-        <v>42821</v>
-      </c>
-      <c r="L4" s="2">
-        <v>42821</v>
-      </c>
-      <c r="M4">
+      <c r="E6" s="2" t="n">
+        <v>42837</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>42857</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>42858</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>42873</v>
+      </c>
+      <c r="J6" t="n">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>42874</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>42886</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="D5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="B7" s="2" t="n">
+        <v>42825</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>42832</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>42835</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>42843</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>42845</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>42852</v>
+      </c>
+      <c r="J7" t="n">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>42853</v>
+      </c>
+      <c r="L7" s="2" t="n">
+        <v>42859</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
todo lo relacionado a los reportes post-DoPlanning estan listos
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Reporte de atrasos</t>
   </si>
@@ -69,7 +69,7 @@
     <t>Empleados encargados instalación</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5 ;1</t>
   </si>
 </sst>
 </file>
@@ -113,11 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +482,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>42831</v>
+        <v>42834</v>
       </c>
       <c r="C4" s="2">
-        <v>42849</v>
+        <v>42843</v>
       </c>
     </row>
   </sheetData>
@@ -496,10 +495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -562,85 +561,40 @@
         <v>42817</v>
       </c>
       <c r="C4" s="2">
-        <v>42823</v>
+        <v>42822</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>42824</v>
+        <v>42823</v>
       </c>
       <c r="F4" s="2">
         <v>42830</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H4" s="2">
         <v>42831</v>
       </c>
       <c r="I4" s="2">
-        <v>42835</v>
+        <v>42836</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4" s="2">
-        <v>42842</v>
+        <v>42837</v>
       </c>
       <c r="L4" s="2">
-        <v>42849</v>
+        <v>42843</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>42824</v>
-      </c>
-      <c r="C5" s="2">
-        <v>42825</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>42831</v>
-      </c>
-      <c r="F5" s="2">
-        <v>42833</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>42833</v>
-      </c>
-      <c r="I5" s="2">
-        <v>42837</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5" s="2">
-        <v>42850</v>
-      </c>
-      <c r="L5" s="2">
-        <v>42855</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="L6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reportes post-planificacion revisados, todo anda bien, archivos costs.py creado
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="330" yWindow="480" windowWidth="19800" windowHeight="7350" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Reporte atrasos" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Reporte planificación" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Reporte atrasos" sheetId="2" r:id="rId2"/>
+    <sheet name="Reporte planificación" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Reporte de atrasos</t>
   </si>
@@ -69,7 +69,13 @@
     <t>Empleados encargados instalación</t>
   </si>
   <si>
-    <t>12 ;13 ;4 ;8</t>
+    <t>4 ;12 ;8 ;13</t>
+  </si>
+  <si>
+    <t>12 ;13</t>
+  </si>
+  <si>
+    <t>4 ;8</t>
   </si>
 </sst>
 </file>
@@ -77,23 +83,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,17 +117,46 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -407,40 +444,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -460,48 +484,44 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="n">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>42865</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>42879</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42889</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42892</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="30"/>
-    <col customWidth="1" max="3" min="3" width="30"/>
-    <col customWidth="1" max="4" min="4" width="30"/>
-    <col customWidth="1" max="5" min="5" width="30"/>
-    <col customWidth="1" max="6" min="6" width="30"/>
-    <col customWidth="1" max="7" min="7" width="30"/>
-    <col customWidth="1" max="8" min="8" width="30"/>
-    <col customWidth="1" max="9" min="9" width="30"/>
-    <col customWidth="1" max="10" min="10" width="30"/>
-    <col customWidth="1" max="11" min="11" width="30"/>
-    <col customWidth="1" max="12" min="12" width="30"/>
-    <col customWidth="1" max="13" min="13" width="30"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="13" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -551,47 +571,170 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="n">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>42851</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>42851</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="B4" s="2">
         <v>42852</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="C4" s="2">
         <v>42852</v>
       </c>
-      <c r="G4" t="n">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42853</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42853</v>
+      </c>
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>42853</v>
-      </c>
-      <c r="I4" s="2" t="n">
-        <v>42859</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="H4" s="2">
+        <v>42857</v>
+      </c>
+      <c r="I4" s="2">
+        <v>42860</v>
+      </c>
+      <c r="J4">
         <v>11</v>
       </c>
-      <c r="K4" s="2" t="n">
+      <c r="K4" s="2">
         <v>42878</v>
       </c>
-      <c r="L4" s="2" t="n">
+      <c r="L4" s="2">
         <v>42879</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42852</v>
+      </c>
+      <c r="C5" s="2">
+        <v>42852</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42853</v>
+      </c>
+      <c r="F5" s="2">
+        <v>42853</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2">
+        <v>42857</v>
+      </c>
+      <c r="I5" s="2">
+        <v>42863</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2">
+        <v>42880</v>
+      </c>
+      <c r="L5" s="2">
+        <v>42885</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42852</v>
+      </c>
+      <c r="C6" s="2">
+        <v>42852</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42853</v>
+      </c>
+      <c r="F6" s="2">
+        <v>42853</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>42857</v>
+      </c>
+      <c r="I6" s="2">
+        <v>42872</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>42880</v>
+      </c>
+      <c r="L6" s="2">
+        <v>42892</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>42852</v>
+      </c>
+      <c r="C7" s="2">
+        <v>42852</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42853</v>
+      </c>
+      <c r="F7" s="2">
+        <v>42853</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>42863</v>
+      </c>
+      <c r="I7" s="2">
+        <v>42870</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2">
+        <v>42886</v>
+      </c>
+      <c r="L7" s="2">
+        <v>42891</v>
+      </c>
+      <c r="M7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
varios cambios hechos a los reportes post-planificacion, esta todo listo en ese lado
</commit_message>
<xml_diff>
--- a/ReportePlanificacion.xlsx
+++ b/ReportePlanificacion.xlsx
@@ -459,7 +459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -491,7 +493,7 @@
         <v>42865</v>
       </c>
       <c r="C4" s="2">
-        <v>42879</v>
+        <v>42906</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -502,7 +504,7 @@
         <v>42889</v>
       </c>
       <c r="C5" s="2">
-        <v>42892</v>
+        <v>42920</v>
       </c>
     </row>
   </sheetData>
@@ -514,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -575,37 +577,37 @@
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="C4" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="F4" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
       <c r="H4" s="2">
-        <v>42857</v>
+        <v>42884</v>
       </c>
       <c r="I4" s="2">
-        <v>42860</v>
+        <v>42887</v>
       </c>
       <c r="J4">
         <v>11</v>
       </c>
       <c r="K4" s="2">
-        <v>42878</v>
+        <v>42905</v>
       </c>
       <c r="L4" s="2">
-        <v>42879</v>
+        <v>42906</v>
       </c>
       <c r="M4" t="s">
         <v>17</v>
@@ -616,37 +618,37 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="C5" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="F5" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
       <c r="H5" s="2">
-        <v>42857</v>
+        <v>42884</v>
       </c>
       <c r="I5" s="2">
-        <v>42863</v>
+        <v>42888</v>
       </c>
       <c r="J5">
         <v>7</v>
       </c>
       <c r="K5" s="2">
-        <v>42880</v>
+        <v>42907</v>
       </c>
       <c r="L5" s="2">
-        <v>42885</v>
+        <v>42913</v>
       </c>
       <c r="M5" t="s">
         <v>19</v>
@@ -657,37 +659,37 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="C6" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="F6" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>42857</v>
+        <v>42884</v>
       </c>
       <c r="I6" s="2">
-        <v>42872</v>
+        <v>42899</v>
       </c>
       <c r="J6">
         <v>3</v>
       </c>
       <c r="K6" s="2">
-        <v>42880</v>
+        <v>42907</v>
       </c>
       <c r="L6" s="2">
-        <v>42892</v>
+        <v>42920</v>
       </c>
       <c r="M6" t="s">
         <v>18</v>
@@ -698,37 +700,37 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="C7" s="2">
-        <v>42852</v>
+        <v>42880</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="F7" s="2">
-        <v>42853</v>
+        <v>42881</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7" s="2">
-        <v>42863</v>
+        <v>42888</v>
       </c>
       <c r="I7" s="2">
-        <v>42870</v>
+        <v>42895</v>
       </c>
       <c r="J7">
         <v>11</v>
       </c>
       <c r="K7" s="2">
-        <v>42886</v>
+        <v>42914</v>
       </c>
       <c r="L7" s="2">
-        <v>42891</v>
+        <v>42919</v>
       </c>
       <c r="M7" t="s">
         <v>19</v>

</xml_diff>